<commit_message>
Added project documentation files
</commit_message>
<xml_diff>
--- a/1. Analysis of the problem/3_диаграмма_паретто.xlsx
+++ b/1. Analysis of the problem/3_диаграмма_паретто.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Анастасия\Desktop\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DNU\Ефимов\1. Analysis of the problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC182F08-860A-49CA-849A-452E324D7A31}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FDE666-5982-415D-9C73-BEC7C6E04B82}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="503" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$D$2:$D$11</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$E$2:$E$11</definedName>
   </definedNames>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -43,41 +43,41 @@
     <t>Порог</t>
   </si>
   <si>
-    <t>Лимитированый доступ к общению</t>
+    <t>Проблемы с авторскими правами на существующих соц. Сетях</t>
   </si>
   <si>
-    <t>Непринятие обществом</t>
+    <t>Проблема поиска юмористических изображений</t>
   </si>
   <si>
-    <t>Проблемы с получением образования</t>
+    <t>Проблема поиска юмористических видео</t>
   </si>
   <si>
-    <t>Неспособность найти работу</t>
+    <t>Проблемы авторов с поиском аудитории</t>
   </si>
   <si>
-    <t>Отсутствие новых знакомств</t>
+    <t>Плохая адаптированость существующих соц. Сетей для мемов</t>
   </si>
   <si>
-    <t>Отрешенность от современного образа жизни</t>
+    <t>Трудности при обсуждении мемов</t>
   </si>
   <si>
-    <t>Ограниченные возможности следить за новостями</t>
+    <t>Неудобство общения в соц. Сетях с видео мемами</t>
   </si>
   <si>
-    <t>Невозможность пользования соцсетями</t>
+    <t>Сложность поиска определенного мема</t>
   </si>
   <si>
-    <t>Отсутствие приложений для людей с дефектами зрения</t>
+    <t>Сложность модификавции мемов</t>
   </si>
   <si>
-    <t>Неполноценность нынешних голосовых помощников</t>
+    <t>Ограниченные возможности следить за новыми мемами</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +229,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{30E17B9B-2BB2-44E3-AABD-6EDC21A8C945}" formatIdx="0">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>Кол-во случаев</cx:v>
             </cx:txData>
           </cx:tx>
@@ -241,6 +242,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{F75BBE73-6F3A-4944-8B5A-80E8C3A985F6}" formatIdx="2">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>Кол-во плохих случаев</cx:v>
             </cx:txData>
           </cx:tx>
@@ -253,6 +255,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{3F43F32A-9E0E-4705-8EC8-7904C382392D}" formatIdx="4">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>Порог</cx:v>
             </cx:txData>
           </cx:tx>
@@ -923,7 +926,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="295275" y="2000250"/>
-              <a:ext cx="7839075" cy="4829175"/>
+              <a:ext cx="8420100" cy="4829175"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -942,7 +945,7 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr sz="1100"/>
+                <a:rPr lang="en-US" sz="1100"/>
                 <a:t>This chart isn't available in your version of Excel.
 Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
               </a:r>
@@ -1255,20 +1258,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.59765625" customWidth="1"/>
     <col min="2" max="2" width="69" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.3984375" customWidth="1"/>
+    <col min="4" max="4" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1286,190 +1289,187 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" s="7">
-        <f>C2/SUM(C2:C10)</f>
-        <v>0.1871345029239766</v>
+        <v>0.32</v>
       </c>
       <c r="E2" s="7">
         <v>0.8</v>
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="7">
         <f>C3/SUM(C2:C10)+D2</f>
-        <v>0.34502923976608185</v>
+        <v>0.46970059880239523</v>
       </c>
       <c r="E3" s="7">
         <v>0.8</v>
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" ref="D4" si="0">C4/SUM(C4:C12)</f>
-        <v>0.21052631578947367</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="E4" s="7">
         <v>0.8</v>
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="7">
-        <f t="shared" ref="D5" si="1">C5/SUM(C4:C12)+D4</f>
-        <v>0.41228070175438591</v>
+        <v>0.22</v>
       </c>
       <c r="E5" s="7">
         <v>0.8</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="7">
-        <f t="shared" ref="D6" si="2">C6/SUM(C6:C14)</f>
-        <v>0.26865671641791045</v>
+        <f t="shared" ref="D6" si="1">C6/SUM(C6:C14)</f>
+        <v>0.23170731707317074</v>
       </c>
       <c r="E6" s="7">
         <v>0.8</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2">
         <v>17</v>
       </c>
       <c r="D7" s="7">
-        <f t="shared" ref="D7" si="3">C7/SUM(C6:C14)+D6</f>
-        <v>0.52238805970149249</v>
+        <f t="shared" ref="D7" si="2">C7/SUM(C6:C14)+D6</f>
+        <v>0.43902439024390244</v>
       </c>
       <c r="E7" s="7">
         <v>0.8</v>
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2">
         <v>15</v>
       </c>
       <c r="D8" s="7">
-        <f t="shared" ref="D8" si="4">C8/SUM(C8:C16)</f>
-        <v>0.46875</v>
+        <f t="shared" ref="D8" si="3">C8/SUM(C8:C16)</f>
+        <v>0.32608695652173914</v>
       </c>
       <c r="E8" s="7">
         <v>0.8</v>
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2">
         <v>9</v>
       </c>
       <c r="D9" s="7">
-        <f t="shared" ref="D9" si="5">C9/SUM(C8:C16)+D8</f>
-        <v>0.75</v>
+        <f t="shared" ref="D9" si="4">C9/SUM(C8:C16)+D8</f>
+        <v>0.52173913043478259</v>
       </c>
       <c r="E9" s="7">
         <v>0.8</v>
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D10" s="7">
-        <f t="shared" ref="D10" si="6">C10/SUM(C10:C18)</f>
-        <v>0.75</v>
+        <f t="shared" ref="D10" si="5">C10/SUM(C10:C18)</f>
+        <v>0.45454545454545453</v>
       </c>
       <c r="E10" s="7">
         <v>0.8</v>
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D11" s="7">
-        <f t="shared" ref="D11" si="7">C11/SUM(C10:C18)+D10</f>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E11" s="7">
         <v>0.8</v>

</xml_diff>